<commit_message>
update with working simulation
</commit_message>
<xml_diff>
--- a/missile_policy_parameters.xlsx
+++ b/missile_policy_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karadowling/Desktop/Independent Work/Missile Code/Missile-Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9EB3E8-EF87-4845-807B-C64D9BA98D25}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBABFD11-FEA3-7A44-8294-4349D47A34FF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" activeTab="1" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>'full_grid' policy is a grid search over theta values using the high_low policy</t>
   </si>
@@ -155,13 +155,16 @@
   <si>
     <t>Defensive Missile Success Probability</t>
   </si>
+  <si>
+    <t>Offensive Missile Success Probability</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#\ ???/???"/>
+    <numFmt numFmtId="164" formatCode="#\ ???/???"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -208,7 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B272AC-B9F0-6245-988D-8924FC3BFAF0}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,10 +623,11 @@
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="6" width="17.1640625" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -645,11 +649,14 @@
       <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -672,10 +679,13 @@
         <v>100</v>
       </c>
       <c r="H2" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="I2" s="3">
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -698,6 +708,9 @@
         <v>300</v>
       </c>
       <c r="H3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="I3" s="3">
         <v>0.16666666666666666</v>
       </c>
     </row>

</xml_diff>